<commit_message>
Finished agenda and tested vs. hardcoded
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_6_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_6_checkers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,6 +523,396 @@
         <v>31</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>100</v>
+      </c>
+      <c r="C24" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>100</v>
+      </c>
+      <c r="C33" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>100</v>
+      </c>
+      <c r="C34" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ran even more tests
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_6_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_6_checkers.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="guerrilla vs. hardcoded COIN 6 checkers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="g vs. hardcoded C 6 checkers" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,6 +913,136 @@
         <v>21</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>100</v>
+      </c>
+      <c r="C39" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+      <c r="C41" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>100</v>
+      </c>
+      <c r="C44" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>